<commit_message>
Finish Risk, Start Return
</commit_message>
<xml_diff>
--- a/FinalProject/Analysis_Carpenter/Example Functions/Portfolio Opt. Real World Data.xlsx
+++ b/FinalProject/Analysis_Carpenter/Example Functions/Portfolio Opt. Real World Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive - University of Oklahoma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\DScourseS20\FinalProject\Analysis_Carpenter\Example Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3551" documentId="8_{B6DB92FA-B744-4E3F-AF42-2725CA60EEF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{62F39A26-58DC-498F-BD23-0CCD0ECA697C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAD32FA-C02A-43BA-8159-48801D693DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6E0FF362-F7E2-4986-8190-DAF7F8611905}"/>
+    <workbookView xWindow="-22597" yWindow="-3773" windowWidth="22695" windowHeight="14596" xr2:uid="{6E0FF362-F7E2-4986-8190-DAF7F8611905}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1392,27 +1392,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF185326-3EE2-4FB5-A2D7-CC74E2DCC064}">
   <dimension ref="A9:AE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P23" workbookViewId="0">
-      <selection activeCell="Z38" sqref="Z38"/>
+    <sheetView tabSelected="1" topLeftCell="H26" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="6" width="8.9296875" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="2.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="6" width="9" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.73046875" customWidth="1"/>
-    <col min="23" max="25" width="10.6640625" customWidth="1"/>
-    <col min="26" max="26" width="20.59765625" customWidth="1"/>
-    <col min="27" max="27" width="36.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="23" max="27" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="9:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="9:31" x14ac:dyDescent="0.25">
       <c r="Z9" s="44" t="s">
         <v>35</v>
       </c>
@@ -1420,7 +1418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I10" s="7" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I12" s="24">
         <v>39052</v>
       </c>
@@ -1568,7 +1566,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I13" s="25">
         <f>EOMONTH(I12,11)+1</f>
         <v>39417</v>
@@ -1634,7 +1632,7 @@
         <v>-2.0558778301284011E-2</v>
       </c>
     </row>
-    <row r="14" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I14" s="25">
         <f t="shared" ref="I14:I24" si="16">EOMONTH(I13,11)+1</f>
         <v>39783</v>
@@ -1700,7 +1698,7 @@
         <v>0.33908719513023616</v>
       </c>
     </row>
-    <row r="15" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I15" s="25">
         <f t="shared" si="16"/>
         <v>40148</v>
@@ -1766,7 +1764,7 @@
         <v>-0.12691781580037059</v>
       </c>
     </row>
-    <row r="16" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="9:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I16" s="25">
         <f t="shared" si="16"/>
         <v>40513</v>
@@ -1832,7 +1830,7 @@
         <v>-3.3725920920937583E-2</v>
       </c>
     </row>
-    <row r="17" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I17" s="25">
         <f t="shared" si="16"/>
         <v>40878</v>
@@ -1898,7 +1896,7 @@
         <v>7.0768775591025276E-2</v>
       </c>
     </row>
-    <row r="18" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I18" s="25">
         <f t="shared" si="16"/>
         <v>41244</v>
@@ -1964,7 +1962,7 @@
         <v>-2.3203092957179441E-2</v>
       </c>
     </row>
-    <row r="19" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I19" s="25">
         <f t="shared" si="16"/>
         <v>41609</v>
@@ -2030,7 +2028,7 @@
         <v>-0.20270748517276843</v>
       </c>
     </row>
-    <row r="20" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I20" s="25">
         <f t="shared" si="16"/>
         <v>41974</v>
@@ -2096,7 +2094,7 @@
         <v>-4.7207585173300551E-2</v>
       </c>
     </row>
-    <row r="21" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I21" s="25">
         <f t="shared" si="16"/>
         <v>42339</v>
@@ -2162,7 +2160,7 @@
         <v>0.20661969877883085</v>
       </c>
     </row>
-    <row r="22" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I22" s="25">
         <f t="shared" si="16"/>
         <v>42705</v>
@@ -2228,7 +2226,7 @@
         <v>-0.201684212764983</v>
       </c>
     </row>
-    <row r="23" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I23" s="25">
         <f t="shared" si="16"/>
         <v>43070</v>
@@ -2294,7 +2292,7 @@
         <v>-9.0969766470366656E-2</v>
       </c>
     </row>
-    <row r="24" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="9:24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I24" s="26">
         <f t="shared" si="16"/>
         <v>43435</v>
@@ -2360,19 +2358,19 @@
         <v>0.13049898806109811</v>
       </c>
     </row>
-    <row r="26" spans="9:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I26" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="43">
+      <c r="J26" s="43" t="e">
         <f>MAX(T36:T1048576)</f>
-        <v>0.81850965667984033</v>
-      </c>
-    </row>
-    <row r="27" spans="9:24" x14ac:dyDescent="0.45">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I27" s="27"/>
     </row>
-    <row r="28" spans="9:24" x14ac:dyDescent="0.45">
+    <row r="28" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I28" s="27"/>
       <c r="J28" s="27" t="s">
         <v>13</v>
@@ -2381,7 +2379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="9:24" x14ac:dyDescent="0.45">
+    <row r="29" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I29" s="28" t="s">
         <v>28</v>
       </c>
@@ -2392,33 +2390,33 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="9:24" x14ac:dyDescent="0.45">
+    <row r="30" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I30" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="36" t="e">
         <f>INDEX($P$37:$T$1048576,MATCH(LARGE($T$37:$T$1048576,1),$T$37:$T$1048576,0),1)</f>
-        <v>0.33247153729429951</v>
-      </c>
-      <c r="K30" s="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="36" t="e">
         <f>INDEX($P$37:$T$1048576,MATCH(LARGE($T$37:$T$1048576,1),$T$37:$T$1048576,0),2)</f>
-        <v>0.29213116384657584</v>
-      </c>
-    </row>
-    <row r="31" spans="9:24" x14ac:dyDescent="0.45">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J31" s="36">
+      <c r="J31" s="36" t="e">
         <f>MAX(P37:P1048576)</f>
-        <v>1.777565853119073</v>
-      </c>
-      <c r="K31" s="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="36" t="e">
         <f>K29+J26*J31</f>
-        <v>1.4749548161622998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I33" s="7" t="s">
         <v>15</v>
       </c>
@@ -2442,7 +2440,7 @@
       <c r="Z33" s="8"/>
       <c r="AA33" s="37"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I34" s="28" t="s">
         <v>10</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>STF</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="V35" s="13" t="str">
         <f t="array" ref="V35:V39">TRANSPOSE(W34:AA34)</f>
         <v>OIL</v>
@@ -2510,7 +2508,7 @@
         <v>-4.1247389738146449E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J36" s="29" t="str">
         <f>J11</f>
         <v>OIL</v>
@@ -2568,7 +2566,7 @@
         <v>3.1823047638038712E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I37" s="28" t="s">
         <v>11</v>
       </c>
@@ -2591,9 +2589,9 @@
         <f t="shared" ref="O37:O47" si="18">SUM(J37:N37)</f>
         <v>1</v>
       </c>
-      <c r="P37" s="36">
-        <f t="array" ref="P37">SQRT(MMULT(MMULT(J37:N37,$W$35:$AA$39),TRANSPOSE(J37:N37)))</f>
-        <v>0.43076338884044785</v>
+      <c r="P37" s="36" t="e">
+        <f>SQRT(MMULT(MMULT(J37:N37,$W$35:$AA$39),TRANSPOSE(J37:N37)))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="Q37" s="36">
         <f t="array" ref="Q37">MMULT(J37:N37,TRANSPOSE($J$34:$N$34))</f>
@@ -2603,9 +2601,9 @@
         <f t="shared" ref="R37:R47" si="19">TEXT(J37*100,"0")&amp;"/"&amp;TEXT(K37*100,"0")&amp;"/"&amp;TEXT(L37*100,"0")&amp;"/"&amp;TEXT(M37*100,"0")&amp;"/"&amp;TEXT(N37*100,"0")</f>
         <v>0/0/100/0/0</v>
       </c>
-      <c r="T37" s="42">
-        <f t="shared" ref="T37:T47" si="20">(Q37-$K$29)/P37</f>
-        <v>-3.3479790548655527E-3</v>
+      <c r="T37" s="42" t="e">
+        <f>(Q37-$K$29)/P37</f>
+        <v>#VALUE!</v>
       </c>
       <c r="V37" s="13" t="str">
         <v>GOLD</v>
@@ -2626,7 +2624,7 @@
         <v>2.1444572118210704E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I38" s="28" t="s">
         <v>11</v>
       </c>
@@ -2665,7 +2663,7 @@
         <v>23</v>
       </c>
       <c r="T38" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q38-$K$29)/P38</f>
         <v>0.3223376205682883</v>
       </c>
       <c r="V38" s="13" t="str">
@@ -2687,7 +2685,7 @@
         <v>2.6113196482852156E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I39" s="28" t="s">
         <v>11</v>
       </c>
@@ -2723,7 +2721,7 @@
         <v>0/0/0/0/100</v>
       </c>
       <c r="T39" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q39-$K$29)/P39</f>
         <v>0.33392111087166892</v>
       </c>
       <c r="V39" s="22" t="str">
@@ -2745,7 +2743,7 @@
         <v>2.4182295719929889E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
@@ -2788,11 +2786,11 @@
         <v>16</v>
       </c>
       <c r="T40" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q40-$K$29)/P40</f>
         <v>0.38806029030997202</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I41" s="28" t="s">
         <v>11</v>
       </c>
@@ -2831,11 +2829,11 @@
         <v>22</v>
       </c>
       <c r="T41" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q41-$K$29)/P41</f>
         <v>0.39673730883272995</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I42" s="28" t="s">
         <v>11</v>
       </c>
@@ -2874,11 +2872,11 @@
         <v>20</v>
       </c>
       <c r="T42" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q42-$K$29)/P42</f>
         <v>0.51732762265540388</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I43" s="28" t="s">
         <v>11</v>
       </c>
@@ -2917,11 +2915,11 @@
         <v>21</v>
       </c>
       <c r="T43" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q43-$K$29)/P43</f>
         <v>0.61484001684268963</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I44" s="28" t="s">
         <v>11</v>
       </c>
@@ -2957,11 +2955,11 @@
         <v>0/100/0/0/0</v>
       </c>
       <c r="T44" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q44-$K$29)/P44</f>
         <v>0.47488152113474202</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>0</v>
       </c>
@@ -3015,11 +3013,11 @@
         <v>6/0/0/48/45</v>
       </c>
       <c r="T45" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q45-$K$29)/P45</f>
         <v>0.81850965667984033</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>38718</v>
       </c>
@@ -3073,11 +3071,11 @@
         <v>100/0/0/0/0</v>
       </c>
       <c r="T46" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q46-$K$29)/P46</f>
         <v>0.2346675177606346</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38749</v>
       </c>
@@ -3134,11 +3132,11 @@
         <v>17</v>
       </c>
       <c r="T47" s="42">
-        <f t="shared" si="20"/>
+        <f>(Q47-$K$29)/P47</f>
         <v>0.76371691721918045</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>38777</v>
       </c>
@@ -3158,7 +3156,7 @@
         <v>32.398994000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>38808</v>
       </c>
@@ -3178,7 +3176,7 @@
         <v>33.014476999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>38838</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>32.485165000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>38869</v>
       </c>
@@ -3218,7 +3216,7 @@
         <v>32.029708999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>38899</v>
       </c>
@@ -3238,7 +3236,7 @@
         <v>32.653961000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>38930</v>
       </c>
@@ -3258,7 +3256,7 @@
         <v>33.518177000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>38961</v>
       </c>
@@ -3278,7 +3276,7 @@
         <v>33.835273999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>38991</v>
       </c>
@@ -3298,7 +3296,7 @@
         <v>34.954407000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>39022</v>
       </c>
@@ -3318,7 +3316,7 @@
         <v>35.426929000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>39052</v>
       </c>
@@ -3338,7 +3336,7 @@
         <v>35.370967999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>39083</v>
       </c>
@@ -3358,7 +3356,7 @@
         <v>36.294620999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>39114</v>
       </c>
@@ -3378,7 +3376,7 @@
         <v>35.898879999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>39142</v>
       </c>
@@ -3398,7 +3396,7 @@
         <v>36.426524999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>39173</v>
       </c>
@@ -3418,7 +3416,7 @@
         <v>37.902678999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>39203</v>
       </c>
@@ -3438,7 +3436,7 @@
         <v>38.901443</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>39234</v>
       </c>
@@ -3458,7 +3456,7 @@
         <v>38.179070000000003</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>39264</v>
       </c>
@@ -3478,7 +3476,7 @@
         <v>37.944664000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>39295</v>
       </c>
@@ -3498,7 +3496,7 @@
         <v>38.775471000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>39326</v>
       </c>
@@ -3518,7 +3516,7 @@
         <v>40.360984999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>39356</v>
       </c>
@@ -3538,7 +3536,7 @@
         <v>41.007880999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>39387</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>40.265861999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>39417</v>
       </c>
@@ -3578,7 +3576,7 @@
         <v>38.642277</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>39448</v>
       </c>
@@ -3598,7 +3596,7 @@
         <v>38.201084000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>39479</v>
       </c>
@@ -3618,7 +3616,7 @@
         <v>38.068461999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>39508</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>38.234240999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>39539</v>
       </c>
@@ -3658,7 +3656,7 @@
         <v>39.460971999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>39569</v>
       </c>
@@ -3678,7 +3676,7 @@
         <v>39.765991</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>39600</v>
       </c>
@@ -3698,7 +3696,7 @@
         <v>36.357674000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>39630</v>
       </c>
@@ -3718,7 +3716,7 @@
         <v>36.288868000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>39661</v>
       </c>
@@ -3738,7 +3736,7 @@
         <v>36.610897000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>39692</v>
       </c>
@@ -3758,7 +3756,7 @@
         <v>34.329844999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>39722</v>
       </c>
@@ -3778,7 +3776,7 @@
         <v>29.378616000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>39753</v>
       </c>
@@ -3798,7 +3796,7 @@
         <v>28.35885</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>39783</v>
       </c>
@@ -3818,7 +3816,7 @@
         <v>28.318595999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39814</v>
       </c>
@@ -3838,7 +3836,7 @@
         <v>26.115518999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>39845</v>
       </c>
@@ -3858,7 +3856,7 @@
         <v>23.622489999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>39873</v>
       </c>
@@ -3878,7 +3876,7 @@
         <v>25.373062000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>39904</v>
       </c>
@@ -3898,7 +3896,7 @@
         <v>26.898845999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>39934</v>
       </c>
@@ -3918,7 +3916,7 @@
         <v>28.472318999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>39965</v>
       </c>
@@ -3938,7 +3936,7 @@
         <v>28.199860000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>39995</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>30.662361000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>40026</v>
       </c>
@@ -3978,7 +3976,7 @@
         <v>31.028386999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>40057</v>
       </c>
@@ -3998,7 +3996,7 @@
         <v>32.216197999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>40087</v>
       </c>
@@ -4018,7 +4016,7 @@
         <v>32.188580000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>40118</v>
       </c>
@@ -4038,7 +4036,7 @@
         <v>33.997936000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>40148</v>
       </c>
@@ -4058,7 +4056,7 @@
         <v>33.949599999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>40179</v>
       </c>
@@ -4078,7 +4076,7 @@
         <v>32.939414999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>40210</v>
       </c>
@@ -4098,7 +4096,7 @@
         <v>33.491199000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>40238</v>
       </c>
@@ -4118,7 +4116,7 @@
         <v>35.230365999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>40269</v>
       </c>
@@ -4138,7 +4136,7 @@
         <v>35.879931999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>40299</v>
       </c>
@@ -4158,7 +4156,7 @@
         <v>32.860591999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>40330</v>
       </c>
@@ -4178,7 +4176,7 @@
         <v>30.994627000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>40360</v>
       </c>
@@ -4198,7 +4196,7 @@
         <v>33.482872</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>40391</v>
       </c>
@@ -4218,7 +4216,7 @@
         <v>32.244858000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>40422</v>
       </c>
@@ -4238,7 +4236,7 @@
         <v>34.812846999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>40452</v>
       </c>
@@ -4258,7 +4256,7 @@
         <v>35.916438999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>40483</v>
       </c>
@@ -4278,7 +4276,7 @@
         <v>35.668830999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>40513</v>
       </c>
@@ -4298,7 +4296,7 @@
         <v>37.536472000000003</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>40544</v>
       </c>
@@ -4318,7 +4316,7 @@
         <v>38.343505999999998</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>40575</v>
       </c>
@@ -4338,7 +4336,7 @@
         <v>39.816882999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>40603</v>
       </c>
@@ -4358,7 +4356,7 @@
         <v>39.788277000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>40634</v>
       </c>
@@ -4378,7 +4376,7 @@
         <v>41.311717999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>40664</v>
       </c>
@@ -4398,7 +4396,7 @@
         <v>40.417675000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>40695</v>
       </c>
@@ -4418,7 +4416,7 @@
         <v>39.416350999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>40725</v>
       </c>
@@ -4438,7 +4436,7 @@
         <v>38.700980999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>40756</v>
       </c>
@@ -4458,7 +4456,7 @@
         <v>36.806080000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>40787</v>
       </c>
@@ -4478,7 +4476,7 @@
         <v>34.173447000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>40817</v>
       </c>
@@ -4498,7 +4496,7 @@
         <v>37.456989</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>40848</v>
       </c>
@@ -4518,7 +4516,7 @@
         <v>37.681198000000002</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>40878</v>
       </c>
@@ -4538,7 +4536,7 @@
         <v>37.579945000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>40909</v>
       </c>
@@ -4558,7 +4556,7 @@
         <v>39.367218000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>40940</v>
       </c>
@@ -4578,7 +4576,7 @@
         <v>40.495334999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>40969</v>
       </c>
@@ -4598,7 +4596,7 @@
         <v>41.161952999999997</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>41000</v>
       </c>
@@ -4618,7 +4616,7 @@
         <v>40.788361000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>41030</v>
       </c>
@@ -4638,7 +4636,7 @@
         <v>38.715243999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>41061</v>
       </c>
@@ -4658,7 +4656,7 @@
         <v>39.858021000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>41091</v>
       </c>
@@ -4678,7 +4676,7 @@
         <v>40.628051999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>41122</v>
       </c>
@@ -4698,7 +4696,7 @@
         <v>40.917461000000003</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>41153</v>
       </c>
@@ -4718,7 +4716,7 @@
         <v>42.075080999999997</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>41183</v>
       </c>
@@ -4738,7 +4736,7 @@
         <v>41.288490000000003</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>41214</v>
       </c>
@@ -4758,7 +4756,7 @@
         <v>41.340434999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>41244</v>
       </c>
@@ -4778,7 +4776,7 @@
         <v>41.154926000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>41275</v>
       </c>
@@ -4798,7 +4796,7 @@
         <v>44.020519</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>41306</v>
       </c>
@@ -4818,7 +4816,7 @@
         <v>44.674956999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>41334</v>
       </c>
@@ -4838,7 +4836,7 @@
         <v>46.044013999999997</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>41365</v>
       </c>
@@ -4858,7 +4856,7 @@
         <v>46.472785999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>41395</v>
       </c>
@@ -4878,7 +4876,7 @@
         <v>47.014389000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>41426</v>
       </c>
@@ -4898,7 +4896,7 @@
         <v>45.901093000000003</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>41456</v>
       </c>
@@ -4918,7 +4916,7 @@
         <v>48.767052</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>41487</v>
       </c>
@@ -4938,7 +4936,7 @@
         <v>46.834319999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>41518</v>
       </c>
@@ -4958,7 +4956,7 @@
         <v>47.876778000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>41548</v>
       </c>
@@ -4978,7 +4976,7 @@
         <v>50.174747000000004</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>41579</v>
       </c>
@@ -4998,7 +4996,7 @@
         <v>51.300891999999997</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>41609</v>
       </c>
@@ -5018,7 +5016,7 @@
         <v>52.457484999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>41640</v>
       </c>
@@ -5038,7 +5036,7 @@
         <v>50.610526999999998</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>41671</v>
       </c>
@@ -5058,7 +5056,7 @@
         <v>52.934792000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>41699</v>
       </c>
@@ -5078,7 +5076,7 @@
         <v>54.066139</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>41730</v>
       </c>
@@ -5098,7 +5096,7 @@
         <v>55.197495000000004</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>41760</v>
       </c>
@@ -5118,7 +5116,7 @@
         <v>55.56691</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>41791</v>
       </c>
@@ -5138,7 +5136,7 @@
         <v>55.944031000000003</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>41821</v>
       </c>
@@ -5158,7 +5156,7 @@
         <v>55.618361999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>41852</v>
       </c>
@@ -5178,7 +5176,7 @@
         <v>57.532215000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>41883</v>
       </c>
@@ -5198,7 +5196,7 @@
         <v>57.718929000000003</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>41913</v>
       </c>
@@ -5218,7 +5216,7 @@
         <v>58.325760000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>41944</v>
       </c>
@@ -5238,7 +5236,7 @@
         <v>59.656120000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>41974</v>
       </c>
@@ -5258,7 +5256,7 @@
         <v>58.706982000000004</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>42005</v>
       </c>
@@ -5278,7 +5276,7 @@
         <v>57.443615000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>42036</v>
       </c>
@@ -5298,7 +5296,7 @@
         <v>60.188763000000002</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>42064</v>
       </c>
@@ -5318,7 +5316,7 @@
         <v>58.961703999999997</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>42095</v>
       </c>
@@ -5338,7 +5336,7 @@
         <v>59.811211</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>42125</v>
       </c>
@@ -5358,7 +5356,7 @@
         <v>60.393276</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>42156</v>
       </c>
@@ -5378,7 +5376,7 @@
         <v>58.285259000000003</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>42186</v>
       </c>
@@ -5398,7 +5396,7 @@
         <v>59.584468999999999</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>42217</v>
       </c>
@@ -5418,7 +5416,7 @@
         <v>56.47316</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>42248</v>
       </c>
@@ -5438,7 +5436,7 @@
         <v>54.857815000000002</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>42278</v>
       </c>
@@ -5458,7 +5456,7 @@
         <v>58.613678</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>42309</v>
       </c>
@@ -5478,7 +5476,7 @@
         <v>58.390869000000002</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>42339</v>
       </c>
@@ -5498,7 +5496,7 @@
         <v>50.799576000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>42370</v>
       </c>
@@ -5518,7 +5516,7 @@
         <v>55.481521999999998</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>42401</v>
       </c>
@@ -5538,7 +5536,7 @@
         <v>55.795132000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>42430</v>
       </c>
@@ -5558,7 +5556,7 @@
         <v>59.334408000000003</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>42461</v>
       </c>
@@ -5578,7 +5576,7 @@
         <v>60.454430000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>42491</v>
       </c>
@@ -5598,7 +5596,7 @@
         <v>61.162289000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>42522</v>
       </c>
@@ -5618,7 +5616,7 @@
         <v>61.628219999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>42552</v>
       </c>
@@ -5638,7 +5636,7 @@
         <v>64.326201999999995</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>42583</v>
       </c>
@@ -5658,7 +5656,7 @@
         <v>63.889842999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>42614</v>
       </c>
@@ -5678,7 +5676,7 @@
         <v>63.462563000000003</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>42644</v>
       </c>
@@ -5698,7 +5696,7 @@
         <v>61.817146000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>42675</v>
       </c>
@@ -5718,7 +5716,7 @@
         <v>64.008018000000007</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>42705</v>
       </c>
@@ -5738,7 +5736,7 @@
         <v>64.698905999999994</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>42736</v>
       </c>
@@ -5758,7 +5756,7 @@
         <v>66.417952999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>42767</v>
       </c>
@@ -5778,7 +5776,7 @@
         <v>68.356414999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>42795</v>
       </c>
@@ -5798,7 +5796,7 @@
         <v>68.597565000000003</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>42826</v>
       </c>
@@ -5818,7 +5816,7 @@
         <v>69.079864999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>42856</v>
       </c>
@@ -5838,7 +5836,7 @@
         <v>69.645638000000005</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>42887</v>
       </c>
@@ -5858,7 +5856,7 @@
         <v>68.931472999999997</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>42917</v>
       </c>
@@ -5878,7 +5876,7 @@
         <v>70.478851000000006</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>42948</v>
       </c>
@@ -5898,7 +5896,7 @@
         <v>70.450691000000006</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>42979</v>
       </c>
@@ -5918,7 +5916,7 @@
         <v>72.130989</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43009</v>
       </c>
@@ -5938,7 +5936,7 @@
         <v>73.341933999999995</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43040</v>
       </c>
@@ -5958,7 +5956,7 @@
         <v>75.482215999999994</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>43070</v>
       </c>
@@ -5978,7 +5976,7 @@
         <v>75.238144000000005</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>43101</v>
       </c>
@@ -5998,7 +5996,7 @@
         <v>79.491569999999996</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43132</v>
       </c>
@@ -6018,7 +6016,7 @@
         <v>75.103119000000007</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>43160</v>
       </c>
@@ -6038,7 +6036,7 @@
         <v>73.393828999999997</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43191</v>
       </c>
@@ -6058,7 +6056,7 @@
         <v>73.009720000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>43221</v>
       </c>
@@ -6078,7 +6076,7 @@
         <v>74.344498000000002</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>43252</v>
       </c>
@@ -6098,7 +6096,7 @@
         <v>74.104423999999995</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43282</v>
       </c>
@@ -6118,7 +6116,7 @@
         <v>78.551270000000002</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43313</v>
       </c>
@@ -6138,7 +6136,7 @@
         <v>79.863861</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>43344</v>
       </c>
@@ -6158,7 +6156,7 @@
         <v>81.011161999999999</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>43374</v>
       </c>
@@ -6178,7 +6176,7 @@
         <v>77.005324999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43405</v>
       </c>
@@ -6198,7 +6196,7 @@
         <v>78.813782000000003</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43435</v>
       </c>
@@ -6218,7 +6216,7 @@
         <v>70.831290999999993</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43466</v>
       </c>
@@ -6238,7 +6236,7 @@
         <v>76.529999000000004</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43497</v>
       </c>
@@ -6258,7 +6256,7 @@
         <v>79.089995999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43525</v>
       </c>
@@ -6278,7 +6276,7 @@
         <v>80.830001999999993</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43556</v>
       </c>
@@ -6298,7 +6296,7 @@
         <v>83.82</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>43586</v>
       </c>

</xml_diff>